<commit_message>
Update contribution sheet and report PDF
</commit_message>
<xml_diff>
--- a/PROJECT FILES/CONTRIBUTION SHEET.XLSX
+++ b/PROJECT FILES/CONTRIBUTION SHEET.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adham Sobhy\Downloads\DATA ANALYSIS GROUP PROJECT\PROJECT FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBBE5A0-4C20-460A-9E8F-AAF54D36DD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2227129-6473-489A-961A-325C1F8630F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,20 +88,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>       Hypotheses 1 &amp; 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>       Data Analysis for hypothesis tests 1 &amp; 2</t>
     </r>
   </si>
@@ -116,20 +102,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>       Hypothesis Testing Steps for hypothesis tests 1 &amp; 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>       Poster</t>
     </r>
   </si>
@@ -240,20 +212,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>       Hypothesis 5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>       Introduction and Conclusion</t>
     </r>
   </si>
@@ -268,20 +226,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>       Data Analysis for hypothesis test 5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>       Hypothesis Testing Steps for hypothesis test 5</t>
     </r>
   </si>
@@ -367,6 +311,62 @@
         <family val="1"/>
       </rPr>
       <t>       Python Notebook Collection and Maintenance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       Hypotheses 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       Hypothesis Testing Steps for hypothesis tests 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>       Hypothesis 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>       Data Analysis for hypothesis test 2</t>
     </r>
   </si>
 </sst>
@@ -532,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -540,28 +540,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -571,19 +565,24 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,19 +866,19 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" style="9" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" style="14" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="9" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="9"/>
-    <col min="9" max="10" width="8.88671875" style="9" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="5" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="10" width="8.88671875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -892,216 +891,216 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="15" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="15" t="s">
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="15" t="s">
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="16" t="s">
+      <c r="D8" s="9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="11">
+      <c r="C18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="15" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="15" t="s">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="16" t="s">
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="15" t="s">
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="11">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="D8:D12"/>
     <mergeCell ref="D18:D22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="D8:D12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>